<commit_message>
added documentation for forgot password and track order test class
</commit_message>
<xml_diff>
--- a/src/resources/testdata/RegistrationTestdata.xlsx
+++ b/src/resources/testdata/RegistrationTestdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam_kushwaha\eclipse-workspace\ShoppingPortal\src\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2841D186-68DC-41A2-A611-56EDA1514CF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824E974A-8FF0-4D04-9DEB-155362DD2135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{876CA80F-7544-4073-996E-2A26EAA3BC1B}"/>
+    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{876CA80F-7544-4073-996E-2A26EAA3BC1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Positve Testdata" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>fullname</t>
   </si>
@@ -52,37 +52,40 @@
     <t>confirm</t>
   </si>
   <si>
-    <t>fake11</t>
-  </si>
-  <si>
-    <t>fake11@g.com</t>
-  </si>
-  <si>
     <t>fake@12345</t>
   </si>
   <si>
     <t>fake12</t>
   </si>
   <si>
-    <t>fake12@g.com</t>
-  </si>
-  <si>
-    <t>fake1</t>
-  </si>
-  <si>
     <t>sk@g.com</t>
   </si>
   <si>
     <t>fake2</t>
   </si>
   <si>
-    <t>new@g.com</t>
-  </si>
-  <si>
-    <t>new@12345</t>
-  </si>
-  <si>
     <t>new@123</t>
+  </si>
+  <si>
+    <t>sk123</t>
+  </si>
+  <si>
+    <t>new@1234</t>
+  </si>
+  <si>
+    <t>new890@g.com</t>
+  </si>
+  <si>
+    <t>fake90</t>
+  </si>
+  <si>
+    <t>fake91</t>
+  </si>
+  <si>
+    <t>fake879@g.com</t>
+  </si>
+  <si>
+    <t>fake456@g.com</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78302F6-17C1-4A9E-A107-C21C676E3316}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,36 +490,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>1267438191</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>3456789012</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -536,11 +539,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B32AF3-6FA8-4495-9880-5133232EE830}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -561,36 +567,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>1234567876</v>
-      </c>
-      <c r="D2">
-        <v>123</v>
-      </c>
-      <c r="E2">
-        <v>123</v>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C3">
         <v>1234567890</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>